<commit_message>
modification on update tarrif file
</commit_message>
<xml_diff>
--- a/Project List.xlsx
+++ b/Project List.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="542">
   <si>
     <t>RSPL</t>
   </si>
@@ -1633,9 +1633,6 @@
     <t>CMT LAB</t>
   </si>
   <si>
-    <t>IVL</t>
-  </si>
-  <si>
     <t>Kolar</t>
   </si>
   <si>
@@ -1652,6 +1649,12 @@
   </si>
   <si>
     <t>Anjuman</t>
+  </si>
+  <si>
+    <t>Indorama</t>
+  </si>
+  <si>
+    <t>Staff Canteen</t>
   </si>
 </sst>
 </file>
@@ -4077,35 +4080,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B915"/>
+  <dimension ref="A1:E914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:XFD70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="65.88671875" style="79" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="79"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" s="50" t="s">
         <v>265</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="52" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="53">
         <v>2.91</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="D2" s="84" t="s">
+        <v>526</v>
+      </c>
+      <c r="E2" s="85">
+        <v>3.47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="52" t="s">
         <v>12</v>
       </c>
@@ -4113,7 +4124,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:5">
       <c r="A4" s="52" t="s">
         <v>183</v>
       </c>
@@ -4121,7 +4132,7 @@
         <v>10.752000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:5">
       <c r="A5" s="52" t="s">
         <v>518</v>
       </c>
@@ -4129,7 +4140,7 @@
         <v>11.01</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:5">
       <c r="A6" s="52" t="s">
         <v>519</v>
       </c>
@@ -4137,7 +4148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:5">
       <c r="A7" s="52" t="s">
         <v>78</v>
       </c>
@@ -4145,7 +4156,7 @@
         <v>15.32</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:5">
       <c r="A8" s="54" t="s">
         <v>3</v>
       </c>
@@ -4153,7 +4164,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:5">
       <c r="A9" s="54" t="s">
         <v>4</v>
       </c>
@@ -4161,7 +4172,7 @@
         <v>6.51</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:5">
       <c r="A10" s="54" t="s">
         <v>5</v>
       </c>
@@ -4169,7 +4180,7 @@
         <v>4.3600000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:5">
       <c r="A11" s="54" t="s">
         <v>6</v>
       </c>
@@ -4177,7 +4188,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:5">
       <c r="A12" s="54" t="s">
         <v>7</v>
       </c>
@@ -4185,7 +4196,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:5">
       <c r="A13" s="54" t="s">
         <v>8</v>
       </c>
@@ -4193,7 +4204,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:5">
       <c r="A14" s="54" t="s">
         <v>520</v>
       </c>
@@ -4201,7 +4212,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:5">
       <c r="A15" s="54" t="s">
         <v>9</v>
       </c>
@@ -4209,7 +4220,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:5">
       <c r="A16" s="54" t="s">
         <v>521</v>
       </c>
@@ -4315,7 +4326,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="80" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B29" s="81">
         <v>3.2</v>
@@ -4642,32 +4653,32 @@
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="84" t="s">
-        <v>526</v>
-      </c>
-      <c r="B70" s="85">
+      <c r="A70" s="60" t="s">
+        <v>296</v>
+      </c>
+      <c r="B70" s="70">
         <v>3.47</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="60" t="s">
-        <v>296</v>
+        <v>527</v>
       </c>
       <c r="B71" s="70">
         <v>3.47</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="60" t="s">
-        <v>527</v>
+      <c r="A72" s="69" t="s">
+        <v>528</v>
       </c>
       <c r="B72" s="70">
         <v>3.47</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="69" t="s">
-        <v>528</v>
+      <c r="A73" s="63" t="s">
+        <v>529</v>
       </c>
       <c r="B73" s="70">
         <v>3.47</v>
@@ -4675,31 +4686,31 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="63" t="s">
-        <v>529</v>
-      </c>
-      <c r="B74" s="70">
+        <v>298</v>
+      </c>
+      <c r="B74" s="61">
         <v>3.47</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="63" t="s">
-        <v>298</v>
-      </c>
-      <c r="B75" s="61">
+        <v>299</v>
+      </c>
+      <c r="B75" s="62">
         <v>3.47</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="63" t="s">
-        <v>299</v>
-      </c>
-      <c r="B76" s="62">
-        <v>3.47</v>
+      <c r="A76" s="71" t="s">
+        <v>300</v>
+      </c>
+      <c r="B76" s="72">
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="71" t="s">
-        <v>300</v>
+        <v>530</v>
       </c>
       <c r="B77" s="72">
         <v>4.1500000000000004</v>
@@ -4707,7 +4718,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="71" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B78" s="72">
         <v>4.1500000000000004</v>
@@ -4715,7 +4726,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="71" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B79" s="72">
         <v>4.1500000000000004</v>
@@ -4723,75 +4734,71 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="71" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B80" s="72">
         <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="71" t="s">
-        <v>533</v>
-      </c>
-      <c r="B81" s="72">
+      <c r="A81" s="73" t="s">
+        <v>541</v>
+      </c>
+      <c r="B81" s="74">
         <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="73" t="s">
-        <v>69</v>
-      </c>
-      <c r="B82" s="74">
+      <c r="A82" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="76">
         <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="B83" s="76">
-        <v>4.1500000000000004</v>
+      <c r="A83" s="86" t="s">
+        <v>539</v>
+      </c>
+      <c r="B83" s="87">
+        <v>5.9</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="86" t="s">
+      <c r="A84" s="75" t="s">
         <v>540</v>
       </c>
-      <c r="B84" s="87">
-        <v>5.9</v>
+      <c r="B84" s="76">
+        <v>4.5</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="75" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="B85" s="76">
-        <v>4.5</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="75" t="s">
+        <v>534</v>
+      </c>
+      <c r="B86" s="76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="60" t="s">
         <v>538</v>
       </c>
-      <c r="B86" s="76">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="75" t="s">
-        <v>535</v>
-      </c>
-      <c r="B87" s="76">
-        <v>4</v>
+      <c r="B87" s="62">
+        <v>3.69</v>
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="60" t="s">
-        <v>539</v>
-      </c>
-      <c r="B88" s="62">
-        <v>3.69</v>
-      </c>
+      <c r="A88" s="77"/>
+      <c r="B88" s="78"/>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="77"/>
@@ -8096,10 +8103,6 @@
     <row r="914" spans="1:2">
       <c r="A914" s="77"/>
       <c r="B914" s="78"/>
-    </row>
-    <row r="915" spans="1:2">
-      <c r="A915" s="77"/>
-      <c r="B915" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>